<commit_message>
arreglos de la parte de excel
</commit_message>
<xml_diff>
--- a/uploads/ExcelPruebaOrangeG55.xlsx
+++ b/uploads/ExcelPruebaOrangeG55.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arodriguez62\ProgramasTFG\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ED0544-CD5F-40EA-B105-C59F20A329E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF15AE4E-34ED-427C-B474-FEB6B9843E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27516" yWindow="2988" windowWidth="23040" windowHeight="12120" xr2:uid="{D6015473-BA1F-4047-BAD7-7918617657AA}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{D6015473-BA1F-4047-BAD7-7918617657AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2023,18 +2023,18 @@
     <t>bug number</t>
   </si>
   <si>
-    <t xml:space="preserve">Raised in
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed in
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed by </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tested by  </t>
+    <t>Raised in
+(Soft. Vers.)</t>
+  </si>
+  <si>
+    <t>Fixed in
+(Soft. Vers.)</t>
+  </si>
+  <si>
+    <t>Fixed by QA or on prototype (prototype by default)</t>
+  </si>
+  <si>
+    <t>Tested by  MCO</t>
   </si>
 </sst>
 </file>
@@ -2804,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDAB574-9F8C-7E41-9BC7-62B769BED3D6}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2877,7 +2877,7 @@
       <c r="L4" s="26"/>
       <c r="M4" s="27"/>
     </row>
-    <row r="5" spans="1:13" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>0</v>
       </c>

</xml_diff>